<commit_message>
feat: calration in teknik
</commit_message>
<xml_diff>
--- a/calibration.xlsx
+++ b/calibration.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihzas\Documents\PlatformIO\Projects\solar-tracker-bap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A81AFD-05AA-4EDD-852E-8A7079467335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC25E72-B80D-4C88-86A3-3E3F9942038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{412789F5-83FC-4300-98EA-ED3E881853AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{412789F5-83FC-4300-98EA-ED3E881853AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>App</t>
   </si>
@@ -5158,8 +5159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B49BD2-EAE6-45E2-84BC-67323D698AA5}">
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5424,4 +5425,281 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E85246-7F43-497E-8FBD-B2CFDEEA594A}">
+  <dimension ref="B3:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>-0.8</v>
+      </c>
+      <c r="D5">
+        <v>0.11</v>
+      </c>
+      <c r="E5">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3.5</v>
+      </c>
+      <c r="C6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D6">
+        <v>2.76</v>
+      </c>
+      <c r="E6">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>6.9</v>
+      </c>
+      <c r="C7">
+        <v>5.6</v>
+      </c>
+      <c r="D7">
+        <v>5.78</v>
+      </c>
+      <c r="E7">
+        <v>-5.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>10.5</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>9.15</v>
+      </c>
+      <c r="E8">
+        <v>-9.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>13.1</v>
+      </c>
+      <c r="C9">
+        <v>11.5</v>
+      </c>
+      <c r="D9">
+        <v>11.8</v>
+      </c>
+      <c r="E9">
+        <v>-11.8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>16.7</v>
+      </c>
+      <c r="C10">
+        <v>14.5</v>
+      </c>
+      <c r="D10">
+        <v>15.15</v>
+      </c>
+      <c r="E10">
+        <v>-14.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>19.8</v>
+      </c>
+      <c r="C11">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D11">
+        <v>18.2</v>
+      </c>
+      <c r="E11">
+        <v>-17.899999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>22.9</v>
+      </c>
+      <c r="C12">
+        <v>20.6</v>
+      </c>
+      <c r="D12">
+        <v>21.2</v>
+      </c>
+      <c r="E12">
+        <v>-20.8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>25.9</v>
+      </c>
+      <c r="C13">
+        <v>23.8</v>
+      </c>
+      <c r="D13">
+        <v>24.15</v>
+      </c>
+      <c r="E13">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>28.4</v>
+      </c>
+      <c r="C14">
+        <v>26.9</v>
+      </c>
+      <c r="D14">
+        <v>26.8</v>
+      </c>
+      <c r="E14">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>31.6</v>
+      </c>
+      <c r="C15">
+        <v>29.4</v>
+      </c>
+      <c r="D15">
+        <v>29.8</v>
+      </c>
+      <c r="E15">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D16">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="E16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D17">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>41.4</v>
+      </c>
+      <c r="D18">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>44.4</v>
+      </c>
+      <c r="D19">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>46.5</v>
+      </c>
+      <c r="D20">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>49.7</v>
+      </c>
+      <c r="D21">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>53.2</v>
+      </c>
+      <c r="D22">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>55.5</v>
+      </c>
+      <c r="D23">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>59</v>
+      </c>
+      <c r="D24">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>61.5</v>
+      </c>
+      <c r="D25">
+        <v>59.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>